<commit_message>
some tweaks/fixes, goal/victory logic
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA00614-2EFB-4784-9282-7D140F6F669C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206357CA-5B92-4743-B43D-C61C7B734A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Key</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Test 2</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +446,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
level 1 tweaks, level 2 stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9BED20-C999-4FAA-995F-74229BDFAC0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB876E8-5AB1-404B-BB8C-76D828A1AE14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Key</t>
   </si>
@@ -56,6 +56,66 @@
   </si>
   <si>
     <t>Mighty Chin Chin: What's the Matter</t>
+  </si>
+  <si>
+    <t>material_clay</t>
+  </si>
+  <si>
+    <t>material_clay_1x2</t>
+  </si>
+  <si>
+    <t>material_clay_1x3</t>
+  </si>
+  <si>
+    <t>material_clay_3x1</t>
+  </si>
+  <si>
+    <t>material_clay_6x1</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Clay 1x2</t>
+  </si>
+  <si>
+    <t>Clay 1x3</t>
+  </si>
+  <si>
+    <t>Clay 3x1</t>
+  </si>
+  <si>
+    <t>Clay 6x1</t>
+  </si>
+  <si>
+    <t>tag_wide</t>
+  </si>
+  <si>
+    <t>tag_tall</t>
+  </si>
+  <si>
+    <t>Wide</t>
+  </si>
+  <si>
+    <t>Tall</t>
+  </si>
+  <si>
+    <t>material_iron_block</t>
+  </si>
+  <si>
+    <t>Iron Block</t>
+  </si>
+  <si>
+    <t>tag_heavy</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>tag_light</t>
+  </si>
+  <si>
+    <t>Light</t>
   </si>
 </sst>
 </file>
@@ -388,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +514,86 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
more level 2 stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB876E8-5AB1-404B-BB8C-76D828A1AE14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F209A1-580A-4E77-A92B-A466D77E80A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -116,6 +116,30 @@
   </si>
   <si>
     <t>Light</t>
+  </si>
+  <si>
+    <t>material_granite_boulder</t>
+  </si>
+  <si>
+    <t>Granite Boulder</t>
+  </si>
+  <si>
+    <t>material_cotton_pillow</t>
+  </si>
+  <si>
+    <t>Cotton Pillow</t>
+  </si>
+  <si>
+    <t>material_rubber_duck</t>
+  </si>
+  <si>
+    <t>Rubber Duck</t>
+  </si>
+  <si>
+    <t>material_oak_branch</t>
+  </si>
+  <si>
+    <t>Oak Branch</t>
   </si>
 </sst>
 </file>
@@ -448,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,6 +618,38 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
more level 4 stuff, bug fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F20AE3D-9ED3-4180-81AD-7614805800D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7A8E69-FC6A-442F-80A6-8FCDE4D151D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>Sink</t>
+  </si>
+  <si>
+    <t>tag_conductive</t>
+  </si>
+  <si>
+    <t>Conductive</t>
+  </si>
+  <si>
+    <t>tag_non_conductive</t>
+  </si>
+  <si>
+    <t>Non-Conductive</t>
   </si>
 </sst>
 </file>
@@ -496,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,97 +624,113 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
option, dialog ui art/layout
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AD227C-69A0-4944-818A-5168F35389E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124E825D-1AC3-42AE-852D-770542FB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Key</t>
   </si>
@@ -176,6 +176,48 @@
   </si>
   <si>
     <t>material_plastic_ball</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
   </si>
 </sst>
 </file>
@@ -508,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,161 +618,217 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B32" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactoring material object ui interface for classify, ui layout for classify
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124E825D-1AC3-42AE-852D-770542FB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0622BE-6EFA-41B9-A2BD-1E092D6BF8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>CLOSE</t>
+  </si>
+  <si>
+    <t>classify</t>
+  </si>
+  <si>
+    <t>CLASSIFY</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,161 +680,169 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
level 4 art/layout, ui icons
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0327E848-E8E8-4C51-9B30-3916FBF98F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116F4BCD-4FD2-46BB-841A-EEFB8687CA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Key</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>VICTORY</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>PLAY</t>
   </si>
 </sst>
 </file>
@@ -592,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,273 +666,281 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>51</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tutorials and explanations
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116F4BCD-4FD2-46BB-841A-EEFB8687CA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEDFC58-D545-4596-8F45-D78F1D748DA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Key</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Test 2</t>
   </si>
   <si>
-    <t>Mighty Chin Chin: What's the Matter</t>
-  </si>
-  <si>
     <t>material_clay</t>
   </si>
   <si>
@@ -250,12 +247,6 @@
     <t>CONTINUE</t>
   </si>
   <si>
-    <t>classifications</t>
-  </si>
-  <si>
-    <t>CLASSIFICATIONS</t>
-  </si>
-  <si>
     <t>victory</t>
   </si>
   <si>
@@ -266,6 +257,261 @@
   </si>
   <si>
     <t>PLAY</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Mighty Chin Chin&lt;/b&gt;\n&lt;size=34&gt;What's the Matter&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>PROPERTIES</t>
+  </si>
+  <si>
+    <t>shapes_sizes</t>
+  </si>
+  <si>
+    <t>Shapes and Sizes</t>
+  </si>
+  <si>
+    <t>level01_intro_1</t>
+  </si>
+  <si>
+    <t>level01_intro_2</t>
+  </si>
+  <si>
+    <t>In order to help the mighty Chin-Chin, we will need to learn how to use a bunch of objects with special properties.</t>
+  </si>
+  <si>
+    <t>By learning the properties of objects, we can use them effectively in many situations.</t>
+  </si>
+  <si>
+    <t>level01_property_1</t>
+  </si>
+  <si>
+    <t>An object has many different properties.</t>
+  </si>
+  <si>
+    <t>level01_property_2</t>
+  </si>
+  <si>
+    <t>Each property of an object tells us its quality and attribute.</t>
+  </si>
+  <si>
+    <t>level01_property_3</t>
+  </si>
+  <si>
+    <t>level01_classify_1</t>
+  </si>
+  <si>
+    <t>Classify means to put objects into groups because of their shared properties.</t>
+  </si>
+  <si>
+    <t>level01_classify_2</t>
+  </si>
+  <si>
+    <t>level01_shape_size_1</t>
+  </si>
+  <si>
+    <t>An object can be made into different shapes and sizes.</t>
+  </si>
+  <si>
+    <t>level01_shape_size_2</t>
+  </si>
+  <si>
+    <t>level01_begin_1</t>
+  </si>
+  <si>
+    <t>Let's go ahead and shape a bunch of clay!</t>
+  </si>
+  <si>
+    <t>level01_begin_2</t>
+  </si>
+  <si>
+    <t>For example, a soft material like clay can be squeezed to become tall, or wide.</t>
+  </si>
+  <si>
+    <t>This allows us to make use of objects without having to guess which is which at any situation!</t>
+  </si>
+  <si>
+    <t>drag_instruction_classify</t>
+  </si>
+  <si>
+    <t>You will be tasked to place them into these groups: tall and wide.</t>
+  </si>
+  <si>
+    <t>Drag and drop the object into the matching group.</t>
+  </si>
+  <si>
+    <t>drag_instruction_play</t>
+  </si>
+  <si>
+    <t>Drag and drop the object to the highlighted area.</t>
+  </si>
+  <si>
+    <t>Click on the group tab to switch to another group.</t>
+  </si>
+  <si>
+    <t>palette_switch_instruction</t>
+  </si>
+  <si>
+    <t>play_instruction</t>
+  </si>
+  <si>
+    <t>Press this button to let the mighty Chin-Chin move.</t>
+  </si>
+  <si>
+    <t>stop_instruction</t>
+  </si>
+  <si>
+    <t>Press this button to go back to placing objects.</t>
+  </si>
+  <si>
+    <t>reset_instruction</t>
+  </si>
+  <si>
+    <t>Press and hold this button to clear out all the objects.</t>
+  </si>
+  <si>
+    <t>level01_play_begin_1</t>
+  </si>
+  <si>
+    <t>For example, we can say that a rubber duck is: lightweight, can float above water, and can block electricity.</t>
+  </si>
+  <si>
+    <t>Look! There's one of the star fragments.</t>
+  </si>
+  <si>
+    <t>level01_play_begin_2</t>
+  </si>
+  <si>
+    <t>Let's go ahead and help the mighty Chin-Chin cross the chasm!</t>
+  </si>
+  <si>
+    <t>level02_intro_1</t>
+  </si>
+  <si>
+    <t>For this part, we will be looking at the weight property of objects.</t>
+  </si>
+  <si>
+    <t>level02_intro_2</t>
+  </si>
+  <si>
+    <t>level02_intro_3</t>
+  </si>
+  <si>
+    <t>level02_light_1</t>
+  </si>
+  <si>
+    <t>One way to determine an object's weight is by using a balance scale.</t>
+  </si>
+  <si>
+    <t>The weight of an object tells us how light or heavy it is.</t>
+  </si>
+  <si>
+    <t>level02_heavy_1</t>
+  </si>
+  <si>
+    <t>level02_begin_1</t>
+  </si>
+  <si>
+    <t>Now let's sort out some objects into two classification: light and heavy!</t>
+  </si>
+  <si>
+    <t>level02_begin_2</t>
+  </si>
+  <si>
+    <t>Remember that an object is light if the left scale goes up, and heavy if the left scale goes down.</t>
+  </si>
+  <si>
+    <t>On this example, we can say a 2 pounds pillow is a lightweight relative to a 20 pounds block.</t>
+  </si>
+  <si>
+    <t>A 40 pounds iron block would be a heavyweight relative to a 20 pounds block.</t>
+  </si>
+  <si>
+    <t>buoyancy</t>
+  </si>
+  <si>
+    <t>Buoyancy</t>
+  </si>
+  <si>
+    <t>level03_intro_1</t>
+  </si>
+  <si>
+    <t>level03_buoyancy_1</t>
+  </si>
+  <si>
+    <t>An object's buoyancy determines wether it moves upwards or downwards in liquid matter, such as water.</t>
+  </si>
+  <si>
+    <t>level03_buoyancy_2</t>
+  </si>
+  <si>
+    <t>Now we will be looking at an object's property called buoyancy.</t>
+  </si>
+  <si>
+    <t>level03_buoyancy_3</t>
+  </si>
+  <si>
+    <t>level03_begin_1</t>
+  </si>
+  <si>
+    <t>Let's go ahead and sort these objects on wether they float or sink!</t>
+  </si>
+  <si>
+    <t>If an object moves downward in water, it sinks.</t>
+  </si>
+  <si>
+    <t>If an object moves upward in water, it floats.</t>
+  </si>
+  <si>
+    <t>level04_intro_1</t>
+  </si>
+  <si>
+    <t>For this final part, we will be looking at the conductive property of objects.</t>
+  </si>
+  <si>
+    <t>level04_intro_2</t>
+  </si>
+  <si>
+    <t>An object's conductivity determines if it can transmit heat, electricity, or sound.</t>
+  </si>
+  <si>
+    <t>level04_conductive_1</t>
+  </si>
+  <si>
+    <t>level04_non_conductive_1</t>
+  </si>
+  <si>
+    <t>As for a granite rock, not so much.</t>
+  </si>
+  <si>
+    <t>level04_begin_1</t>
+  </si>
+  <si>
+    <t>level04_begin_2</t>
+  </si>
+  <si>
+    <t>If enough electricity conducts through an object, the light bulb should shine brightly.</t>
+  </si>
+  <si>
+    <t>Here we see that an iron block is highly conductive with electricity.</t>
+  </si>
+  <si>
+    <t>Now let's go ahead and sort these objects on wether they are electrically conductive or not!</t>
   </si>
 </sst>
 </file>
@@ -598,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +891,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,282 +912,610 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
         <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial build, some gameplay tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9833B1-1AD1-4B65-9594-8AA48A2A829F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BBB86-B3D3-4928-93AB-4F287E3A7382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,9 +385,6 @@
     <t>level01_play_begin_1</t>
   </si>
   <si>
-    <t>For example, we can say that a rubber duck is: lightweight, can float above water, and can block electricity.</t>
-  </si>
-  <si>
     <t>Look! There's one of the star fragments.</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>level02_begin_1</t>
   </si>
   <si>
-    <t>Now let's sort out some objects into two classification: light and heavy!</t>
-  </si>
-  <si>
     <t>level02_begin_2</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>level03_buoyancy_1</t>
   </si>
   <si>
-    <t>An object's buoyancy determines wether it moves upwards or downwards in liquid matter, such as water.</t>
-  </si>
-  <si>
     <t>level03_buoyancy_2</t>
   </si>
   <si>
@@ -524,6 +515,15 @@
   </si>
   <si>
     <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>For example, we can say that a rubber duck is: lightweight, floats on water, and can block electricity.</t>
+  </si>
+  <si>
+    <t>Now let's sort out some objects into two classifications: light and heavy!</t>
+  </si>
+  <si>
+    <t>An object's buoyancy determines wether it moves upward or downward in liquid matter, such as water.</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1367,183 +1367,183 @@
         <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
         <v>123</v>
-      </c>
-      <c r="B62" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
         <v>125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>143</v>
+      </c>
+      <c r="B74" t="s">
         <v>146</v>
-      </c>
-      <c r="B74" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated LoL API to v5, added 'continue' and 'new game'; refactor lol stuff to use save state
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BBB86-B3D3-4928-93AB-4F287E3A7382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510FBA48-73FC-479A-AB00-166F2E585548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Key</t>
   </si>
@@ -253,12 +253,6 @@
     <t>VICTORY</t>
   </si>
   <si>
-    <t>play</t>
-  </si>
-  <si>
-    <t>PLAY</t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -524,6 +518,18 @@
   </si>
   <si>
     <t>An object's buoyancy determines wether it moves upward or downward in liquid matter, such as water.</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>Written by: David Dionisio</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>new_game</t>
   </si>
 </sst>
 </file>
@@ -856,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,452 +909,452 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
         <v>103</v>
@@ -1356,175 +1362,175 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" t="s">
         <v>140</v>
-      </c>
-      <c r="B72" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
         <v>144</v>
-      </c>
-      <c r="B75" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B77" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s">
         <v>157</v>
@@ -1532,18 +1538,26 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
go to edit mode after death, change reset to confirm, disable reset if no spawned objects
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510FBA48-73FC-479A-AB00-166F2E585548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DED5E30-D2AB-4BE6-BFCC-9F24216E994F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>Key</t>
   </si>
@@ -370,12 +370,6 @@
     <t>Press this button to go back to placing objects.</t>
   </si>
   <si>
-    <t>reset_instruction</t>
-  </si>
-  <si>
-    <t>Press and hold this button to clear out all the objects.</t>
-  </si>
-  <si>
     <t>level01_play_begin_1</t>
   </si>
   <si>
@@ -530,6 +524,24 @@
   </si>
   <si>
     <t>new_game</t>
+  </si>
+  <si>
+    <t>clear_objects_confirm</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Do you want to remove all the objects placed in the world?</t>
   </si>
 </sst>
 </file>
@@ -862,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,15 +921,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,10 +950,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1282,167 +1294,167 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B67" t="s">
         <v>126</v>
-      </c>
-      <c r="B67" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B70" t="s">
         <v>132</v>
@@ -1450,47 +1462,47 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
         <v>143</v>
@@ -1498,66 +1510,82 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B83" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>162</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added score system, changed placement area graphics
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DED5E30-D2AB-4BE6-BFCC-9F24216E994F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009148EA-2AD5-4AED-B8F8-B23C83A91417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Key</t>
   </si>
@@ -542,6 +542,36 @@
   </si>
   <si>
     <t>Do you want to remove all the objects placed in the world?</t>
+  </si>
+  <si>
+    <t>score_level_complete</t>
+  </si>
+  <si>
+    <t>Level Complete:</t>
+  </si>
+  <si>
+    <t>score_retry_penalty</t>
+  </si>
+  <si>
+    <t>Retry Penalty:</t>
+  </si>
+  <si>
+    <t>score_hint_penalty</t>
+  </si>
+  <si>
+    <t>Hint Penalty:</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Score:</t>
+  </si>
+  <si>
+    <t>score_total</t>
+  </si>
+  <si>
+    <t>Total Score:</t>
   </si>
 </sst>
 </file>
@@ -874,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,273 +1348,313 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B78" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>148</v>
+      </c>
+      <c r="B86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>149</v>
+      </c>
+      <c r="B87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>157</v>
+      </c>
+      <c r="B90" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>159</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B91" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated texts, adjusted level 4 section 3 play
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009148EA-2AD5-4AED-B8F8-B23C83A91417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE862F-DBF8-4047-975B-8BA299DA19CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,66 +283,39 @@
     <t>level01_intro_2</t>
   </si>
   <si>
-    <t>In order to help the mighty Chin-Chin, we will need to learn how to use a bunch of objects with special properties.</t>
-  </si>
-  <si>
-    <t>By learning the properties of objects, we can use them effectively in many situations.</t>
-  </si>
-  <si>
     <t>level01_property_1</t>
   </si>
   <si>
-    <t>An object has many different properties.</t>
-  </si>
-  <si>
     <t>level01_property_2</t>
   </si>
   <si>
-    <t>Each property of an object tells us its quality and attribute.</t>
-  </si>
-  <si>
     <t>level01_property_3</t>
   </si>
   <si>
     <t>level01_classify_1</t>
   </si>
   <si>
-    <t>Classify means to put objects into groups because of their shared properties.</t>
-  </si>
-  <si>
     <t>level01_classify_2</t>
   </si>
   <si>
     <t>level01_shape_size_1</t>
   </si>
   <si>
-    <t>An object can be made into different shapes and sizes.</t>
-  </si>
-  <si>
     <t>level01_shape_size_2</t>
   </si>
   <si>
     <t>level01_begin_1</t>
   </si>
   <si>
-    <t>Let's go ahead and shape a bunch of clay!</t>
-  </si>
-  <si>
     <t>level01_begin_2</t>
   </si>
   <si>
     <t>For example, a soft material like clay can be squeezed to become tall, or wide.</t>
   </si>
   <si>
-    <t>This allows us to make use of objects without having to guess which is which at any situation!</t>
-  </si>
-  <si>
     <t>drag_instruction_classify</t>
   </si>
   <si>
-    <t>You will be tasked to place them into these groups: tall and wide.</t>
-  </si>
-  <si>
     <t>Drag and drop the object into the matching group.</t>
   </si>
   <si>
@@ -373,21 +346,12 @@
     <t>level01_play_begin_1</t>
   </si>
   <si>
-    <t>Look! There's one of the star fragments.</t>
-  </si>
-  <si>
     <t>level01_play_begin_2</t>
   </si>
   <si>
-    <t>Let's go ahead and help the mighty Chin-Chin cross the chasm!</t>
-  </si>
-  <si>
     <t>level02_intro_1</t>
   </si>
   <si>
-    <t>For this part, we will be looking at the weight property of objects.</t>
-  </si>
-  <si>
     <t>level02_intro_2</t>
   </si>
   <si>
@@ -397,12 +361,6 @@
     <t>level02_light_1</t>
   </si>
   <si>
-    <t>One way to determine an object's weight is by using a balance scale.</t>
-  </si>
-  <si>
-    <t>The weight of an object tells us how light or heavy it is.</t>
-  </si>
-  <si>
     <t>level02_heavy_1</t>
   </si>
   <si>
@@ -412,15 +370,6 @@
     <t>level02_begin_2</t>
   </si>
   <si>
-    <t>Remember that an object is light if the left scale goes up, and heavy if the left scale goes down.</t>
-  </si>
-  <si>
-    <t>On this example, we can say a 2 pounds pillow is a lightweight relative to a 20 pounds block.</t>
-  </si>
-  <si>
-    <t>A 40 pounds iron block would be a heavyweight relative to a 20 pounds block.</t>
-  </si>
-  <si>
     <t>buoyancy</t>
   </si>
   <si>
@@ -436,30 +385,15 @@
     <t>level03_buoyancy_2</t>
   </si>
   <si>
-    <t>Now we will be looking at an object's property called buoyancy.</t>
-  </si>
-  <si>
     <t>level03_buoyancy_3</t>
   </si>
   <si>
     <t>level03_begin_1</t>
   </si>
   <si>
-    <t>Let's go ahead and sort these objects on wether they float or sink!</t>
-  </si>
-  <si>
-    <t>If an object moves downward in water, it sinks.</t>
-  </si>
-  <si>
-    <t>If an object moves upward in water, it floats.</t>
-  </si>
-  <si>
     <t>level04_intro_1</t>
   </si>
   <si>
-    <t>For this final part, we will be looking at the conductive property of objects.</t>
-  </si>
-  <si>
     <t>level04_intro_2</t>
   </si>
   <si>
@@ -472,48 +406,24 @@
     <t>level04_non_conductive_1</t>
   </si>
   <si>
-    <t>As for a granite rock, not so much.</t>
-  </si>
-  <si>
     <t>level04_begin_1</t>
   </si>
   <si>
     <t>level04_begin_2</t>
   </si>
   <si>
-    <t>If enough electricity conducts through an object, the light bulb should shine brightly.</t>
-  </si>
-  <si>
-    <t>Here we see that an iron block is highly conductive with electricity.</t>
-  </si>
-  <si>
-    <t>Now let's go ahead and sort these objects on wether they are electrically conductive or not!</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Mighty Chin-Chin&lt;/b&gt;\n&lt;size=34&gt;What's the Matter&lt;/size&gt;</t>
   </si>
   <si>
     <t>end_title</t>
   </si>
   <si>
-    <t>CONGRATULATIONS</t>
-  </si>
-  <si>
     <t>end_text</t>
   </si>
   <si>
     <t>Thank you for playing!</t>
   </si>
   <si>
-    <t>For example, we can say that a rubber duck is: lightweight, floats on water, and can block electricity.</t>
-  </si>
-  <si>
-    <t>Now let's sort out some objects into two classifications: light and heavy!</t>
-  </si>
-  <si>
-    <t>An object's buoyancy determines wether it moves upward or downward in liquid matter, such as water.</t>
-  </si>
-  <si>
     <t>credits</t>
   </si>
   <si>
@@ -572,6 +482,96 @@
   </si>
   <si>
     <t>Total Score:</t>
+  </si>
+  <si>
+    <t>CONGRATULATIONS!</t>
+  </si>
+  <si>
+    <t>Now, let's go ahead and sort these objects on whether they are electrically conductive or not!</t>
+  </si>
+  <si>
+    <t>To help the mighty Chin-Chin, we need to learn how to use objects with special properties.</t>
+  </si>
+  <si>
+    <t>Each object has properties that fit different tasks.</t>
+  </si>
+  <si>
+    <t>Objects have many different properties.</t>
+  </si>
+  <si>
+    <t>Each property tells us its quality and attribute.</t>
+  </si>
+  <si>
+    <t>For example, a rubber duck is: lightweight, not very strong, floats on water, and can block electricity.</t>
+  </si>
+  <si>
+    <t>Classify means putting objects into groups with shared properties.</t>
+  </si>
+  <si>
+    <t>This allows us to use the right object for every task!</t>
+  </si>
+  <si>
+    <t>Objects can be different shapes and sizes.</t>
+  </si>
+  <si>
+    <t>Let's go ahead and shape clay!</t>
+  </si>
+  <si>
+    <t>Place the clay into two groups: tall and wide.</t>
+  </si>
+  <si>
+    <t>Look! There's a star fragment.</t>
+  </si>
+  <si>
+    <t>Let's help the mighty Chin-Chin cross the deadly pit!</t>
+  </si>
+  <si>
+    <t>Now we will look at the weight property of objects.</t>
+  </si>
+  <si>
+    <t>An object's weight tells us how light or heavy it is.</t>
+  </si>
+  <si>
+    <t>You can determine an object's weight with a balance scale.</t>
+  </si>
+  <si>
+    <t>Here, a 2-pound pillow is light compared to a 20-pound block.</t>
+  </si>
+  <si>
+    <t>A 40-pound iron block is heavycompared to a 20-pound block.</t>
+  </si>
+  <si>
+    <t>Now let's sort objects into two classifications: light and heavy!</t>
+  </si>
+  <si>
+    <t>An object is light if the left scale goes up, and heavy if the left scale goes down.</t>
+  </si>
+  <si>
+    <t>Now let's look at buoyancy.</t>
+  </si>
+  <si>
+    <t>An object's buoyancy determines whether it floats or sinks in water.</t>
+  </si>
+  <si>
+    <t>If an object moves up in water, it floats.</t>
+  </si>
+  <si>
+    <t>If an object moves down in water, it sinks.</t>
+  </si>
+  <si>
+    <t>Sort the objects on whether they float or sink!</t>
+  </si>
+  <si>
+    <t>The final mission! We learn about the conductive property.</t>
+  </si>
+  <si>
+    <t>The iron block is highly conductive with electricity. It lets electricity flow through it very easily.</t>
+  </si>
+  <si>
+    <t>The granite rock is not conductive.</t>
+  </si>
+  <si>
+    <t>Sort these objects by electrically conductive or not!</t>
   </si>
 </sst>
 </file>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,15 +951,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,10 +980,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,106 +1284,106 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,236 +1399,236 @@
         <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B78" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B80" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="B86" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B87" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
         <v>155</v>
@@ -1636,26 +1636,26 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some tweaks to level 2-2, tweaked rubber duck collision, text tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE862F-DBF8-4047-975B-8BA299DA19CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6609884B-FF79-4321-826F-137B072736AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -493,9 +493,6 @@
     <t>To help the mighty Chin-Chin, we need to learn how to use objects with special properties.</t>
   </si>
   <si>
-    <t>Each object has properties that fit different tasks.</t>
-  </si>
-  <si>
     <t>Objects have many different properties.</t>
   </si>
   <si>
@@ -508,9 +505,6 @@
     <t>Classify means putting objects into groups with shared properties.</t>
   </si>
   <si>
-    <t>This allows us to use the right object for every task!</t>
-  </si>
-  <si>
     <t>Objects can be different shapes and sizes.</t>
   </si>
   <si>
@@ -520,9 +514,6 @@
     <t>Place the clay into two groups: tall and wide.</t>
   </si>
   <si>
-    <t>Look! There's a star fragment.</t>
-  </si>
-  <si>
     <t>Let's help the mighty Chin-Chin cross the deadly pit!</t>
   </si>
   <si>
@@ -538,40 +529,49 @@
     <t>Here, a 2-pound pillow is light compared to a 20-pound block.</t>
   </si>
   <si>
-    <t>A 40-pound iron block is heavycompared to a 20-pound block.</t>
-  </si>
-  <si>
-    <t>Now let's sort objects into two classifications: light and heavy!</t>
-  </si>
-  <si>
     <t>An object is light if the left scale goes up, and heavy if the left scale goes down.</t>
   </si>
   <si>
-    <t>Now let's look at buoyancy.</t>
-  </si>
-  <si>
     <t>An object's buoyancy determines whether it floats or sinks in water.</t>
   </si>
   <si>
-    <t>If an object moves up in water, it floats.</t>
-  </si>
-  <si>
-    <t>If an object moves down in water, it sinks.</t>
-  </si>
-  <si>
     <t>Sort the objects on whether they float or sink!</t>
   </si>
   <si>
-    <t>The final mission! We learn about the conductive property.</t>
-  </si>
-  <si>
     <t>The iron block is highly conductive with electricity. It lets electricity flow through it very easily.</t>
   </si>
   <si>
-    <t>The granite rock is not conductive.</t>
-  </si>
-  <si>
     <t>Sort these objects by electrically conductive or not!</t>
+  </si>
+  <si>
+    <t>Now, let's sort objects into two classifications: light and heavy!</t>
+  </si>
+  <si>
+    <t>Now, let's look at buoyancy.</t>
+  </si>
+  <si>
+    <t>A 40-pound iron block is heavy compared to a 20-pound block.</t>
+  </si>
+  <si>
+    <t>The final mission! We will learn about the conductive property.</t>
+  </si>
+  <si>
+    <t>Look! There's a star piece.</t>
+  </si>
+  <si>
+    <t>Each object has properties that fit different jobs.</t>
+  </si>
+  <si>
+    <t>This allows us to use the right object for every job!</t>
+  </si>
+  <si>
+    <t>If an object has a lot of buoyancy, it will move up and float above water.</t>
+  </si>
+  <si>
+    <t>The granite rock, on the other hand, is not conductive. The electricity is unable to flow through at all.</t>
+  </si>
+  <si>
+    <t>If an object has no buoyancy, it will move down and sink under water.</t>
   </si>
 </sst>
 </file>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
         <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
         <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
         <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>107</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1495,7 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,7 +1503,7 @@
         <v>110</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1511,7 +1511,7 @@
         <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1519,7 +1519,7 @@
         <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1535,7 +1535,7 @@
         <v>114</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,7 +1543,7 @@
         <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1567,7 +1567,7 @@
         <v>119</v>
       </c>
       <c r="B80" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
         <v>120</v>
       </c>
       <c r="B81" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
         <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
         <v>126</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>